<commit_message>
Progress report started. Need to do accuracy of parallel version, timing for both, and explanation of where to go.
</commit_message>
<xml_diff>
--- a/serialData/Data.xlsx
+++ b/serialData/Data.xlsx
@@ -90,10 +90,10 @@
     <t>Cv</t>
   </si>
   <si>
-    <t>XA (A-Rich)</t>
+    <t>1-Rich Phase</t>
   </si>
   <si>
-    <t>XA (B-Rich)</t>
+    <t>2-Rich Phase</t>
   </si>
 </sst>
 </file>
@@ -376,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085478472"/>
-        <c:axId val="2085481432"/>
+        <c:axId val="2134516760"/>
+        <c:axId val="2126402440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085478472"/>
+        <c:axId val="2134516760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -388,28 +388,109 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Temperature (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="0"/>
+                  <a:t>kT</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085481432"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126402440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.25"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085481432"/>
+        <c:axId val="2126402440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Heat</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> Capacity (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
+                  <a:t>dE/dT</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085478472"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2134516760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="40000.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -502,7 +583,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>XA (A-Rich)</c:v>
+                  <c:v>1-Rich Phase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -608,7 +689,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>XA (B-Rich)</c:v>
+                  <c:v>2-Rich Phase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -751,27 +832,74 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095341096"/>
-        <c:axId val="2096066104"/>
+        <c:axId val="2080057304"/>
+        <c:axId val="2131002904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095341096"/>
+        <c:axId val="2080057304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Mole</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> Fraction of Species 1 (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
+                  <a:t>X</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="0" baseline="-25000"/>
+                  <a:t>1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2096066104"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2131002904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2096066104"/>
+        <c:axId val="2131002904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -779,24 +907,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
+                  <a:t>kT</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095341096"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2080057304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -850,8 +1021,8 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -872,6 +1043,167 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1017758" cy="261610"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5981700" y="1866900"/>
+          <a:ext cx="1017758" cy="261610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Liquid Mixture</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="949430" cy="261610"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6032500" y="2565400"/>
+          <a:ext cx="949430" cy="261610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Solid Mixture</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1226392" cy="261610"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="3670300"/>
+          <a:ext cx="1226392" cy="261610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Two</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Phase Region</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -884,11 +1216,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pdInfo" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pdInfo_ARich" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pdInfo_ARich" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pdInfo" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1216,7 +1548,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1615,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1780,6 +2112,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>